<commit_message>
fix: sequence names in SB26-AB339
</commit_message>
<xml_diff>
--- a/testdata/SB26-AB339/amp_batches.xlsx
+++ b/testdata/SB26-AB339/amp_batches.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fdb589/Desktop/SB26-subset/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fdb589/GitHub/matq007/test-datasets/testdata/SB26-AB339/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9733EFBE-B886-3B43-B94D-75C0140752DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91469F9-D9AB-B542-BDAE-F041BE53F73A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3740" yWindow="1700" windowWidth="23260" windowHeight="13180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,9 +63,6 @@
     <t>AB339</t>
   </si>
   <si>
-    <t>SB26</t>
-  </si>
-  <si>
     <t>TECH_ES</t>
   </si>
   <si>
@@ -76,6 +73,9 @@
   </si>
   <si>
     <t>Mars_2</t>
+  </si>
+  <si>
+    <t>SB26_AB339</t>
   </si>
 </sst>
 </file>
@@ -405,7 +405,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -420,7 +420,7 @@
     <col min="8" max="8" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -451,10 +451,10 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -463,16 +463,22 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>13</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{6a2630e2-1ac5-455e-8217-0156b1936a76}" enabled="1" method="Standard" siteId="{a3927f91-cda1-4696-af89-8c9f1ceffa91}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>